<commit_message>
data-content-category v0.1.1: fix wrong IRIs, add tree
</commit_message>
<xml_diff>
--- a/data-content-category/data-content-category.xlsx
+++ b/data-content-category/data-content-category.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rupprechtconsultde.sharepoint.com/sites/NAPCOREallpartners/Shared Documents/SubWG4.4/Work Items/Work Item 4.4.2.4 Draft specification/Controlled Vocabs/new vocabs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{20E17BF2-9EC7-364A-BFD8-03464B5AD98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C6EAFEA-D89A-4CE5-B22C-420EBBABF19E}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{20E17BF2-9EC7-364A-BFD8-03464B5AD98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20F92C51-2AFD-4799-8A4A-81332121AC80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="147">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -73,9 +73,6 @@
     <t>owl:versionInfo</t>
   </si>
   <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
     <t>owl:versionIRI</t>
   </si>
   <si>
@@ -196,15 +193,9 @@
     <t>Car parking locations and conditions</t>
   </si>
   <si>
-    <t xml:space="preserve">Car parking availability </t>
-  </si>
-  <si>
     <t>Service and rest area locations and conditions</t>
   </si>
   <si>
-    <t>Service and rest area  availability</t>
-  </si>
-  <si>
     <t>Truck parking locations and conditions</t>
   </si>
   <si>
@@ -370,9 +361,6 @@
     <t>Timetables static</t>
   </si>
   <si>
-    <t>Planned interchanges between  scheduled services</t>
-  </si>
-  <si>
     <t>Hours of operation</t>
   </si>
   <si>
@@ -470,6 +458,24 @@
   </si>
   <si>
     <t>Real-time estimated departure and arrival times</t>
+  </si>
+  <si>
+    <t>owl:priorVersion</t>
+  </si>
+  <si>
+    <t>0.1.1</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.0</t>
+  </si>
+  <si>
+    <t>Planned interchanges between scheduled services</t>
+  </si>
+  <si>
+    <t>Car parking availability</t>
+  </si>
+  <si>
+    <t>Service and rest area availability</t>
   </si>
 </sst>
 </file>
@@ -902,7 +908,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -910,23 +916,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.44140625" customWidth="1"/>
-    <col min="2" max="2" width="87.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="77.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="89.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="77.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -935,7 +941,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -944,7 +950,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -953,7 +959,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -962,7 +968,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -971,7 +977,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -980,1274 +986,1283 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.0</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.1</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="184.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="str">
+        <f t="shared" ref="A18:A46" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B18,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-category</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="str">
-        <f t="shared" ref="A17:A45" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B17,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-category</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14" t="str">
-        <f>CONCATENATE(A19,", ",A33,", ",A41,", ",A46,", ",A55,", ",A60,", ",A64,", ",A74,", ",A77,", ",A81,", ",A90,", ",A96,", ",A118,", ",A26,", ",A30,", ",A126,", ",A139,", ",A140,", ",A141)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/toll-information, https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-, https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information, https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel, https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
-      </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-sub-category</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="14" t="str">
-        <f>CONCATENATE(D19,", ",D33,", ",D41,", ",D46,", ",D55,", ",D60,", ",D64,", ",D74,", ",D77,", ",D81,", ",D90,", ",D96,", ",D118,", ",D26,", ",D30,", ",D126)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability-, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area--availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between--scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information, https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+        <f>CONCATENATE(A20,", ",A34,", ",A42,", ",A47,", ",A56,", ",A61,", ",A65,", ",A75,", ",A78,", ",A82,", ",A91,", ",A97,", ",A119,", ",A27,", ",A31,", ",A127,", ",A140,", ",A141,", ",A142)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/toll-information, https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-, https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information, https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel, https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="str">
         <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-sub-category</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14" t="str">
+        <f>CONCATENATE(D20,", ",D34,", ",D42,", ",D47,", ",D56,", ",D61,", ",D65,", ",D75,", ",D78,", ",D82,", ",D91,", ",D97,", ",D119,", ",D27,", ",D31,", ",D127)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information, https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>CONCATENATE(A21,", ",A22,", ",A23,", ",A24,", ",A25,", ",A26)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="1" t="str">
-        <f>CONCATENATE(A20,", ",A21,", ",A22,", ",A23,", ",A24,", ",A25)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry</v>
-      </c>
-      <c r="B20" s="7" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-width</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-width</v>
-      </c>
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes</v>
-      </c>
-      <c r="B22" s="7" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/gradients</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/gradients</v>
-      </c>
-      <c r="B23" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/junctions</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/junctions</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="D27" s="1" t="str">
+        <f>CONCATENATE(A28,", ",A29,", ",A30)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="1" t="str">
-        <f>CONCATENATE(A27,", ",A28,", ",A29)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character</v>
-      </c>
-      <c r="B27" s="8" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes</v>
-      </c>
-      <c r="B28" s="8" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
-      </c>
-      <c r="B29" s="8" t="s">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data</v>
-      </c>
-      <c r="B30" s="9" t="s">
+      <c r="D31" s="1" t="str">
+        <f>CONCATENATE(A32,", ",A33)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="1" t="str">
-        <f>CONCATENATE(A31,", ",A32)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry</v>
-      </c>
-      <c r="B31" s="15" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
-      </c>
-      <c r="B32" s="15" t="s">
+    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations</v>
-      </c>
-      <c r="B33" s="9" t="s">
+      <c r="D34" s="1" t="str">
+        <f>CONCATENATE(A35,", ",A36,", ",A37,", ",A38,", ",A39,", ",A40,", ",A41)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="1" t="str">
-        <f>CONCATENATE(A34,", ",A35,", ",A36,", ",A37,", ",A38,", ",A39,", ",A40)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions</v>
-      </c>
-      <c r="B34" s="8" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions</v>
-      </c>
-      <c r="B35" s="8" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits</v>
-      </c>
-      <c r="B36" s="8" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs</v>
-      </c>
-      <c r="B37" s="8" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions</v>
-      </c>
-      <c r="B38" s="8" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations</v>
-      </c>
-      <c r="B39" s="8" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
-      </c>
-      <c r="B40" s="8" t="s">
+    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/toll-information</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/toll-information</v>
-      </c>
-      <c r="B41" s="9" t="s">
+      <c r="D42" s="1" t="str">
+        <f>CONCATENATE(A43,", ",A44,", ",A45,", ",A46)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="1" t="str">
-        <f>CONCATENATE(A42,", ",A43,", ",A44,", ",A45)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations</v>
-      </c>
-      <c r="B42" s="8" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads</v>
-      </c>
-      <c r="B43" s="8" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods</v>
-      </c>
-      <c r="B44" s="8" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
-      </c>
-      <c r="B45" s="8" t="s">
+    <row r="47" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="str">
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="141.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B46,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information</v>
-      </c>
-      <c r="B46" s="9" t="s">
+      <c r="D47" s="1" t="str">
+        <f>CONCATENATE(A48,", ",A49,", ",A50,", ",A51,", ",A52,", ",A53,", ",A54,", ",A55)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="str">
+        <f t="shared" ref="A48:A111" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="1" t="str">
-        <f>CONCATENATE(A47,", ",A48,", ",A49,", ",A50,", ",A51,", ",A52,", ",A53,", ",A54)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability-, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area--availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="str">
-        <f t="shared" ref="A47:A110" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions</v>
-      </c>
-      <c r="B47" s="8" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability-</v>
-      </c>
-      <c r="B48" s="8" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions</v>
-      </c>
-      <c r="B49" s="8" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area--availability</v>
-      </c>
-      <c r="B50" s="8" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions</v>
-      </c>
-      <c r="B51" s="8" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability</v>
-      </c>
-      <c r="B52" s="8" t="s">
+    <row r="56" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations</v>
+      </c>
+      <c r="B56" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops</v>
-      </c>
-      <c r="B53" s="8" t="s">
+      <c r="D56" s="1" t="str">
+        <f>CONCATENATE(A57,", ",A58,", ",A59,", ",A60)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
-      </c>
-      <c r="B54" s="8" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations</v>
-      </c>
-      <c r="B55" s="9" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="1" t="str">
-        <f>CONCATENATE(A56,", ",A57,", ",A58,", ",A59)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points</v>
-      </c>
-      <c r="B56" s="8" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations</v>
-      </c>
-      <c r="B57" s="8" t="s">
+    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles</v>
-      </c>
-      <c r="B58" s="8" t="s">
+      <c r="D61" s="1" t="str">
+        <f>CONCATENATE(A62,", ",A63,", ",A64)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
-      </c>
-      <c r="B59" s="8" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics</v>
-      </c>
-      <c r="B60" s="9" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D60" s="1" t="str">
-        <f>CONCATENATE(A61,", ",A62,", ",A63)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations</v>
-      </c>
-      <c r="B61" s="8" t="s">
+    </row>
+    <row r="65" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas</v>
-      </c>
-      <c r="B62" s="8" t="s">
+      <c r="D65" s="1" t="str">
+        <f>CONCATENATE(A66,", ",A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73,", ",A74)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
-      </c>
-      <c r="B63" s="8" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-</v>
-      </c>
-      <c r="B64" s="9" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D64" s="1" t="str">
-        <f>CONCATENATE(A65,", ",A66,", ",A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-</v>
-      </c>
-      <c r="B65" s="8" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-</v>
-      </c>
-      <c r="B66" s="8" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-</v>
-      </c>
-      <c r="B67" s="8" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-</v>
-      </c>
-      <c r="B68" s="8" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations</v>
-      </c>
-      <c r="B69" s="8" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
-      </c>
-      <c r="B70" s="8" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits</v>
-      </c>
-      <c r="B71" s="8" t="s">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="D75" s="1" t="str">
+        <f>CONCATENATE(A76,", ",A77)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
-      </c>
-      <c r="B73" s="8" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information</v>
-      </c>
-      <c r="B74" s="9" t="s">
+    <row r="78" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D74" s="1" t="str">
-        <f>CONCATENATE(A75,", ",A76)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works</v>
-      </c>
-      <c r="B75" s="8" t="s">
+      <c r="D78" s="1" t="str">
+        <f>CONCATENATE(A79,", ",A80,", ",A81)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
-      </c>
-      <c r="B76" s="8" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions</v>
-      </c>
-      <c r="B77" s="9" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D77" s="1" t="str">
-        <f>CONCATENATE(A78,", ",A79,", ",A80)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents</v>
-      </c>
-      <c r="B78" s="8" t="s">
+    </row>
+    <row r="82" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data</v>
+      </c>
+      <c r="B82" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions</v>
-      </c>
-      <c r="B79" s="8" t="s">
+      <c r="D82" s="1" t="str">
+        <f>CONCATENATE(A83,", ",A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89,", ",A90)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
-      </c>
-      <c r="B80" s="8" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data</v>
-      </c>
-      <c r="B81" s="9" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D81" s="1" t="str">
-        <f>CONCATENATE(A82,", ",A83,", ",A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume</v>
-      </c>
-      <c r="B82" s="8" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed</v>
-      </c>
-      <c r="B83" s="8" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times</v>
+      </c>
+      <c r="B87" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues</v>
-      </c>
-      <c r="B84" s="8" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times</v>
-      </c>
-      <c r="B85" s="8" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states</v>
+      </c>
+      <c r="B89" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times</v>
-      </c>
-      <c r="B86" s="8" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays</v>
-      </c>
-      <c r="B87" s="8" t="s">
+    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states</v>
-      </c>
-      <c r="B88" s="8" t="s">
+      <c r="D91" s="1" t="str">
+        <f>CONCATENATE(A92,", ",A93,", ",A94,", ",A95,", ",A96)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
-      </c>
-      <c r="B89" s="8" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-</v>
-      </c>
-      <c r="B90" s="9" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D90" s="1" t="str">
-        <f>CONCATENATE(A91,", ",A92,", ",A93,", ",A94,", ",A95)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers</v>
-      </c>
-      <c r="B91" s="8" t="s">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places</v>
-      </c>
-      <c r="B92" s="8" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest</v>
-      </c>
-      <c r="B93" s="8" t="s">
+    <row r="97" spans="1:4" ht="312.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors</v>
-      </c>
-      <c r="B94" s="8" t="s">
+      <c r="D97" s="1" t="str">
+        <f>CONCATENATE(A98,", ",A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117,", ",A118)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
-      </c>
-      <c r="B95" s="8" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="312.89999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport</v>
-      </c>
-      <c r="B96" s="9" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features</v>
+      </c>
+      <c r="B100" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D96" s="1" t="str">
-        <f>CONCATENATE(A97,", ",A98,", ",A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between--scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features</v>
-      </c>
-      <c r="B97" s="8" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout</v>
-      </c>
-      <c r="B98" s="8" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features</v>
-      </c>
-      <c r="B99" s="8" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/connection-links</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility</v>
-      </c>
-      <c r="B100" s="8" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar</v>
-      </c>
-      <c r="B101" s="8" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/connection-links</v>
-      </c>
-      <c r="B102" s="8" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines</v>
-      </c>
-      <c r="B103" s="8" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators</v>
-      </c>
-      <c r="B104" s="8" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static</v>
-      </c>
-      <c r="B105" s="8" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between--scheduled-services</v>
-      </c>
-      <c r="B107" s="8" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="10" t="str">
+        <f t="shared" ref="A112:A142" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B112,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation</v>
-      </c>
-      <c r="B108" s="8" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details</v>
-      </c>
-      <c r="B109" s="8" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="10" t="str">
-        <f t="shared" si="1"/>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <f>CONCATENATE(A120,", ",A121,", ",A122,", ",A123,", ",A124,", ",A125,", ",A126)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/fares</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="10" t="str">
+        <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="10" t="str">
-        <f t="shared" ref="A111:A141" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B111,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A118" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D118" s="1" t="str">
-        <f>CONCATENATE(A119,", ",A120,", ",A121,", ",A122,", ",A123,", ",A124,", ",A125)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations</v>
-      </c>
-      <c r="B121" s="8" t="s">
+      <c r="B126" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services</v>
+      </c>
+      <c r="B127" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/fares</v>
-      </c>
-      <c r="B122" s="8" t="s">
+      <c r="D127" s="1" t="str">
+        <f>CONCATENATE(A128,", ",A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A136,", ",A137,", ",A138,", ",A139)</f>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options</v>
-      </c>
-      <c r="B123" s="8" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles</v>
-      </c>
-      <c r="B124" s="8" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="10" t="str">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
       </c>
-      <c r="B125" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D126" s="1" t="str">
-        <f>CONCATENATE(A127,", ",A128,", ",A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A130,", ",A137,", ",A138)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations</v>
-      </c>
-      <c r="B128" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations</v>
-      </c>
-      <c r="B129" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability</v>
-      </c>
-      <c r="B134" s="8" t="s">
+      <c r="B139" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel</v>
+      </c>
+      <c r="B140" s="9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability</v>
-      </c>
-      <c r="B135" s="8" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies</v>
+      </c>
+      <c r="B141" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability</v>
-      </c>
-      <c r="B136" s="8" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
+      </c>
+      <c r="B142" s="9" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://w3id.org/mobilitydcat-ap/data-content-category" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2260,7 +2275,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data-content-category v0.1.2: fix wrong IRIs
</commit_message>
<xml_diff>
--- a/data-content-category/data-content-category.xlsx
+++ b/data-content-category/data-content-category.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rupprechtconsultde.sharepoint.com/sites/NAPCOREallpartners/Shared Documents/SubWG4.4/Work Items/Work Item 4.4.2.4 Draft specification/Controlled Vocabs/new vocabs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{20E17BF2-9EC7-364A-BFD8-03464B5AD98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20F92C51-2AFD-4799-8A4A-81332121AC80}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7958C98-C72D-49E2-AF9C-1ACA89798A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -235,21 +235,6 @@
     <t>Availability of delivery areas</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamic traffic signs and regulations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Road closures and access conditions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane closures and access conditions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridge closures and access conditions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunnel closures and access conditions </t>
-  </si>
-  <si>
     <t>Other access restrictions and traffic regulations</t>
   </si>
   <si>
@@ -463,12 +448,6 @@
     <t>owl:priorVersion</t>
   </si>
   <si>
-    <t>0.1.1</t>
-  </si>
-  <si>
-    <t>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.0</t>
-  </si>
-  <si>
     <t>Planned interchanges between scheduled services</t>
   </si>
   <si>
@@ -476,6 +455,27 @@
   </si>
   <si>
     <t>Service and rest area availability</t>
+  </si>
+  <si>
+    <t>Dynamic traffic signs and regulations</t>
+  </si>
+  <si>
+    <t>Road closures and access conditions</t>
+  </si>
+  <si>
+    <t>Lane closures and access conditions</t>
+  </si>
+  <si>
+    <t>Bridge closures and access conditions</t>
+  </si>
+  <si>
+    <t>Tunnel closures and access conditions</t>
+  </si>
+  <si>
+    <t>0.1.2</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.1</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -918,21 +918,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.42578125" customWidth="1"/>
-    <col min="2" max="2" width="87.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="109.109375" customWidth="1"/>
+    <col min="2" max="2" width="87.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="77.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -941,7 +941,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -959,7 +959,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -968,7 +968,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -986,47 +986,47 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.1</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/0.1.2</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1035,12 +1035,12 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="184.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="str">
         <f t="shared" ref="A18:A46" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B18,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-category</v>
@@ -1068,11 +1068,11 @@
       <c r="C18" s="13"/>
       <c r="D18" s="14" t="str">
         <f>CONCATENATE(A20,", ",A34,", ",A42,", ",A47,", ",A56,", ",A61,", ",A65,", ",A75,", ",A78,", ",A82,", ",A91,", ",A97,", ",A119,", ",A27,", ",A31,", ",A127,", ",A140,", ",A141,", ",A142)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/toll-information, https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-, https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information, https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel, https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/toll-information, https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information, https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel, https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/data-content-sub-category</v>
@@ -1083,11 +1083,11 @@
       <c r="C19" s="13"/>
       <c r="D19" s="14" t="str">
         <f>CONCATENATE(D20,", ",D34,", ",D42,", ",D47,", ",D56,", ",D61,", ",D65,", ",D75,", ",D78,", ",D82,", ",D91,", ",D97,", ",D119,", ",D27,", ",D31,", ",D127)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information, https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information, https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
       </c>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-road-network-data</v>
@@ -1100,7 +1100,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry, https://w3id.org/mobilitydcat-ap/data-content-category/road-width, https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/gradients, https://w3id.org/mobilitydcat-ap/data-content-category/junctions, https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/geometry</v>
@@ -1109,7 +1109,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-width</v>
@@ -1118,7 +1118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/number-of-lanes</v>
@@ -1127,7 +1127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/gradients</v>
@@ -1136,7 +1136,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/junctions</v>
@@ -1145,7 +1145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-classification</v>
@@ -1154,7 +1154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/cycle-network-data</v>
@@ -1167,7 +1167,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-geometry-and-lane-character</v>
@@ -1176,7 +1176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-detailed-attributes</v>
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-closures-diversions</v>
@@ -1194,7 +1194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-data</v>
@@ -1207,7 +1207,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-network-geometry</v>
@@ -1216,7 +1216,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/pedestrian-accessibility-facilities</v>
@@ -1225,7 +1225,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/static-traffic-signs-and-regulations</v>
@@ -1238,7 +1238,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-access-conditions</v>
@@ -1247,7 +1247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-access-conditions</v>
@@ -1256,7 +1256,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed-limits</v>
@@ -1265,7 +1265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-static-traffic-signs</v>
@@ -1274,7 +1274,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/permanent-access-restrictions</v>
@@ -1283,7 +1283,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-traffic-regulations</v>
@@ -1292,7 +1292,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-circulation-plans</v>
@@ -1301,7 +1301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/toll-information</v>
@@ -1314,7 +1314,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-tolling-stations</v>
@@ -1323,7 +1323,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/identification-of-tolled-roads</v>
@@ -1332,7 +1332,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/applicable-road-user-charges-and-payment-methods</v>
@@ -1341,7 +1341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods-for-tolls</v>
@@ -1350,7 +1350,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="141.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="str">
         <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/parking-service-and-rest-area-information</v>
@@ -1363,7 +1363,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability, https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="str">
         <f t="shared" ref="A48:A111" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-locations-and-conditions</v>
@@ -1372,16 +1372,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-parking-availability</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-locations-and-conditions</v>
@@ -1390,16 +1390,16 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-and-rest-area-availability</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-locations-and-conditions</v>
@@ -1408,7 +1408,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/truck-parking-availability</v>
@@ -1417,7 +1417,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/park-and-ride-stops</v>
@@ -1426,7 +1426,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-parking-locations</v>
@@ -1435,7 +1435,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/filling-and-charging-stations</v>
@@ -1448,7 +1448,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-charging-points</v>
@@ -1457,7 +1457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-conditions-of-filling-stations</v>
@@ -1466,7 +1466,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-charging-points-for-electric-vehicles</v>
@@ -1475,7 +1475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-filling-stations</v>
@@ -1484,7 +1484,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-and-logistics</v>
@@ -1497,7 +1497,7 @@
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/freight-delivery-regulations</v>
@@ -1506,7 +1506,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-of-delivery-areas</v>
@@ -1515,7 +1515,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/availability-of-delivery-areas</v>
@@ -1524,738 +1524,738 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations-</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-traffic-signs-and-regulations</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="D65" s="1" t="str">
         <f>CONCATENATE(A66,", ",A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73,", ",A74)</f>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions-</v>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-closures-and-access-conditions</v>
       </c>
       <c r="B66" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/lane-closures-and-access-conditions-</v>
-      </c>
-      <c r="B67" s="8" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bridge-closures-and-access-conditions-</v>
-      </c>
-      <c r="B68" s="8" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/tunnel-closures-and-access-conditions-</v>
-      </c>
-      <c r="B69" s="8" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-access-restrictions-and-traffic-regulations</v>
-      </c>
-      <c r="B70" s="8" t="s">
+    <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/dynamic-speed-limits</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/direction-of-travel-on-reversible-lanes</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other-temporary-traffic-management-measures-or-plans</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-work-information</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="D75" s="1" t="str">
         <f>CONCATENATE(A76,", ",A77)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works, https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/long-term-road-works</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/short-term-road-works</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-events-and-conditions</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D78" s="1" t="str">
         <f>CONCATENATE(A79,", ",A80,", ",A81)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/accidents-and-incidents</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/poor-road-conditions</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/road-weather-conditions</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-traffic-data</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D82" s="1" t="str">
         <f>CONCATENATE(A83,", ",A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89,", ",A90)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume, https://w3id.org/mobilitydcat-ap/data-content-category/speed, https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times, https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays, https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-volume</v>
       </c>
       <c r="B83" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/speed</v>
-      </c>
-      <c r="B84" s="8" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states</v>
+      </c>
+      <c r="B89" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/location-and-length-of-queues</v>
-      </c>
-      <c r="B85" s="8" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/current-travel-times</v>
-      </c>
-      <c r="B86" s="8" t="s">
+    <row r="91" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/predicted-travel-times</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/expected-delays</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waiting-time-at-border-crossings-to-non-eu-member-states</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/traffic-data-at-border-crossings-to-third-countries</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/general-information-for-trip-planning-</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="D91" s="1" t="str">
         <f>CONCATENATE(A92,", ",A93,", ",A94,", ",A95,", ",A96)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers, https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places, https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/address-identifiers</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="312.89999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/topographic-places</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/points-of-interest</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-environmental-factors</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/parameters-needed-to-calculate-costs</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="312.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-scheduled-transport</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="D97" s="1" t="str">
         <f>CONCATENATE(A98,", ",A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117,", ",A118)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar, https://w3id.org/mobilitydcat-ap/data-content-category/connection-links, https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators, https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static, https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation, https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes, https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products, https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-location-and-features</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/connection-links</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-geometry-and-map-layout</v>
-      </c>
-      <c r="B99" s="8" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-status-of-features</v>
-      </c>
-      <c r="B100" s="8" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/stop-facilities-accessibility-and-paths-within-facility</v>
-      </c>
-      <c r="B101" s="8" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/operational-calendar</v>
-      </c>
-      <c r="B102" s="8" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/connection-links</v>
-      </c>
-      <c r="B103" s="8" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/network-topology-and-routes-lines</v>
-      </c>
-      <c r="B104" s="8" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/transport-operators</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/timetables-static</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/real-time-estimated-departure-and-arrival-times</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/planned-interchanges-between-scheduled-services</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/hours-of-operation</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/vehicle-details</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="str">
         <f t="shared" ref="A112:A142" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B112,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/disruptions-delays-cancellations</v>
       </c>
       <c r="B112" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-common-standard-fares</v>
-      </c>
-      <c r="B113" s="8" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/passenger-classes</v>
-      </c>
-      <c r="B114" s="8" t="s">
+    <row r="119" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A119" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport</v>
+      </c>
+      <c r="B119" s="9" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/common-fare-products</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/special-fare-products</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/basic-commercial-conditions</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/purchase-information</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/public-transport-non-scheduled-transport</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="D119" s="1" t="str">
         <f>CONCATENATE(A120,", ",A121,", ",A122,", ",A123,", ",A124,", ",A125,", ",A126)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data, https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/fares, https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/provider-data</v>
       </c>
       <c r="B120" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/fares</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles</v>
+      </c>
+      <c r="B125" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/service-areas-and-service-times</v>
-      </c>
-      <c r="B121" s="8" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services</v>
+      </c>
+      <c r="B127" s="9" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/locations-and-stations</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/fares</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/reservation-and-purchase-options</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/accesibility-information-for-vehicles</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B126" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/sharing-and-hiring-services</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D127" s="1" t="str">
         <f>CONCATENATE(A128,", ",A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A136,", ",A137,", ",A138,", ",A139)</f>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods, https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-locations-and-stations</v>
       </c>
       <c r="B128" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability</v>
+      </c>
+      <c r="B133" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-locations-and-stations</v>
-      </c>
-      <c r="B129" s="8" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability</v>
+      </c>
+      <c r="B134" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-stations</v>
-      </c>
-      <c r="B130" s="8" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability</v>
+      </c>
+      <c r="B135" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-stations</v>
-      </c>
-      <c r="B131" s="8" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability</v>
+      </c>
+      <c r="B136" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-locations-and-stations</v>
-      </c>
-      <c r="B132" s="8" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability</v>
+      </c>
+      <c r="B137" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-sharing-availability</v>
-      </c>
-      <c r="B133" s="8" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods</v>
+      </c>
+      <c r="B138" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-sharing-availability</v>
-      </c>
-      <c r="B134" s="8" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel</v>
+      </c>
+      <c r="B140" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/car-hiring-availability</v>
-      </c>
-      <c r="B135" s="8" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies</v>
+      </c>
+      <c r="B141" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/bike-hiring-availability</v>
-      </c>
-      <c r="B136" s="8" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
+      </c>
+      <c r="B142" s="9" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/e-scooter-sharing-availability</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/payment-methods</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/air-and-space-travel</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/waterways-and-water-bodies</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/data-content-category/other</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2263,9 +2263,10 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://w3id.org/mobilitydcat-ap/data-content-category" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
     <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{04893DF2-E013-4FB8-AD83-ADCFBFBA54B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2275,7 +2276,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2545,15 +2546,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
@@ -2564,6 +2556,15 @@
     <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2586,14 +2587,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F704F36C-6F34-42D8-A9E1-097741891E9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2602,4 +2595,12 @@
     <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>